<commit_message>
REV 1 - WIP
Fixed D3, it was the wrong way around
Fixed Q6, Q7, Q8, D and S were the wrong way around
</commit_message>
<xml_diff>
--- a/pcb/bom/samd21_gps_tracker.xlsx
+++ b/pcb/bom/samd21_gps_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acea/projects/hardware/project_samd21_gps_nbiot_lora_tracker/pcb/bom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808A1292-A1D0-FB4D-A83A-34F5B4A69D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD51DD15-996A-9940-8ED3-0714E9960C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{62B02246-6A2E-B541-B52A-AF0A4A7A4A29}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="160">
   <si>
     <t>References</t>
   </si>
@@ -511,6 +511,9 @@
   </si>
   <si>
     <t>C88373</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -862,15 +865,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8535DE91-6916-2D44-8460-64D71BCCCBC3}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -886,8 +892,11 @@
       <c r="F1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -906,8 +915,11 @@
       <c r="F2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -926,8 +938,11 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -946,8 +961,11 @@
       <c r="F4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -966,8 +984,11 @@
       <c r="F5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -986,8 +1007,11 @@
       <c r="F6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1006,8 +1030,11 @@
       <c r="F7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1026,8 +1053,11 @@
       <c r="F8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1046,8 +1076,11 @@
       <c r="F9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1066,8 +1099,11 @@
       <c r="F10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1086,8 +1122,11 @@
       <c r="F11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1106,8 +1145,11 @@
       <c r="F12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1126,8 +1168,11 @@
       <c r="F13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1146,8 +1191,11 @@
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1166,8 +1214,11 @@
       <c r="F15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1186,8 +1237,11 @@
       <c r="F16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1206,8 +1260,11 @@
       <c r="F17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1226,8 +1283,11 @@
       <c r="F18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1246,8 +1306,11 @@
       <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1266,8 +1329,11 @@
       <c r="F20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1286,8 +1352,11 @@
       <c r="F21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1306,8 +1375,11 @@
       <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1326,8 +1398,11 @@
       <c r="F23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1346,8 +1421,11 @@
       <c r="F24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1366,8 +1444,11 @@
       <c r="F25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1383,8 +1464,11 @@
       <c r="F26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1400,8 +1484,11 @@
       <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1420,8 +1507,11 @@
       <c r="F28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1440,8 +1530,11 @@
       <c r="F29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1460,8 +1553,11 @@
       <c r="F30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1480,8 +1576,11 @@
       <c r="F31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1500,8 +1599,11 @@
       <c r="F32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1520,8 +1622,11 @@
       <c r="F33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1540,8 +1645,11 @@
       <c r="F34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1560,8 +1668,11 @@
       <c r="F35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1580,8 +1691,11 @@
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1600,8 +1714,11 @@
       <c r="F37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1620,8 +1737,11 @@
       <c r="F38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1640,8 +1760,11 @@
       <c r="F39">
         <v>6</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1660,8 +1783,11 @@
       <c r="F40">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1680,8 +1806,11 @@
       <c r="F41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1700,8 +1829,11 @@
       <c r="F42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1720,8 +1852,11 @@
       <c r="F43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1740,8 +1875,11 @@
       <c r="F44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1760,8 +1898,11 @@
       <c r="F45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1779,6 +1920,9 @@
       </c>
       <c r="F46">
         <v>2</v>
+      </c>
+      <c r="G46">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>